<commit_message>
da minha parte não há mto mais a fazer (sem ser proteções), agr preciso da tua parte para continuar @raul (votos e assim)
</commit_message>
<xml_diff>
--- a/sd_checklist_meta1.xlsx
+++ b/sd_checklist_meta1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raul/Home/Git/SDIST/projeto_meta_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao_\Documents\João Filipe\Universidade\4º Ano\2º Semestre\SD\Projeto-SD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B47E2457-C877-954C-BF21-10717C010B88}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C132699-3C22-4F2D-803A-7F502C08C37D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="460" windowWidth="26020" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2016-2017" sheetId="2" r:id="rId1"/>
@@ -278,7 +278,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -288,6 +288,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -458,7 +464,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -487,162 +493,165 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="155">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Hiperligação Visitada" xfId="154" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -985,27 +994,27 @@
   </sheetPr>
   <dimension ref="A1:C90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="5" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="27.1640625" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="27.19921875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.5" style="5" customWidth="1"/>
-    <col min="2" max="2" width="66.33203125" style="2" customWidth="1"/>
-    <col min="3" max="16384" width="27.1640625" style="5"/>
+    <col min="2" max="2" width="66.296875" style="2" customWidth="1"/>
+    <col min="3" max="16384" width="27.19921875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="2" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="1.95" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:3" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
         <v>2</v>
       </c>
@@ -1013,7 +1022,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>3</v>
       </c>
@@ -1021,7 +1030,7 @@
         <v>2017987654</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" s="4" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <f>A6+A25+A33+A40</f>
         <v>100</v>
@@ -1034,7 +1043,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <f>SUM(A7:A24)</f>
         <v>44</v>
@@ -1047,51 +1056,51 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>1</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="12" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="5">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>3</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="12" t="s">
         <v>39</v>
       </c>
       <c r="C8" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>3</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="12" t="s">
         <v>38</v>
       </c>
       <c r="C9" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>3</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="12" t="s">
         <v>30</v>
       </c>
       <c r="C10" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>3</v>
       </c>
@@ -1102,7 +1111,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>3</v>
       </c>
@@ -1113,7 +1122,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>3</v>
       </c>
@@ -1124,7 +1133,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>3</v>
       </c>
@@ -1135,18 +1144,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>3</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="12" t="s">
         <v>29</v>
       </c>
       <c r="C15" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>3</v>
       </c>
@@ -1157,7 +1166,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>3</v>
       </c>
@@ -1168,7 +1177,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>3</v>
       </c>
@@ -1179,7 +1188,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>7</v>
       </c>
@@ -1190,7 +1199,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>3</v>
       </c>
@@ -1201,7 +1210,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>0</v>
       </c>
@@ -1212,7 +1221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="5">
         <v>0</v>
       </c>
@@ -1223,7 +1232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="5">
         <v>0</v>
       </c>
@@ -1234,7 +1243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="10">
         <v>0</v>
       </c>
@@ -1245,7 +1254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <f>SUM(A26:A32)</f>
         <v>24</v>
@@ -1258,7 +1267,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="5">
         <v>4</v>
       </c>
@@ -1269,7 +1278,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>4</v>
       </c>
@@ -1280,7 +1289,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>4</v>
       </c>
@@ -1291,7 +1300,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="5">
         <v>4</v>
       </c>
@@ -1302,7 +1311,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="10">
         <v>4</v>
       </c>
@@ -1313,7 +1322,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="10">
         <v>4</v>
       </c>
@@ -1324,7 +1333,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="10">
         <v>0</v>
       </c>
@@ -1335,7 +1344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <f>SUM(A34:A39)</f>
         <v>24</v>
@@ -1348,7 +1357,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="5">
         <v>4</v>
       </c>
@@ -1359,7 +1368,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>4</v>
       </c>
@@ -1370,7 +1379,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>4</v>
       </c>
@@ -1381,7 +1390,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="10">
         <v>4</v>
       </c>
@@ -1392,7 +1401,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>4</v>
       </c>
@@ -1403,7 +1412,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="5">
         <v>4</v>
       </c>
@@ -1414,7 +1423,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <f>SUM(A41:A44)</f>
         <v>8</v>
@@ -1427,7 +1436,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>2</v>
       </c>
@@ -1438,7 +1447,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>2</v>
       </c>
@@ -1449,7 +1458,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>2</v>
       </c>
@@ -1460,7 +1469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="10">
         <v>2</v>
       </c>
@@ -1471,7 +1480,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B45" s="1" t="s">
         <v>8</v>
       </c>
@@ -1480,27 +1489,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B46" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B47" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B48" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B49" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="2:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B50" s="1" t="s">
         <v>9</v>
       </c>
@@ -1509,125 +1518,125 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B51" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B52" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B53" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B54" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B55" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="2:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B56" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B57" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B58" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B59" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B60" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B61" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B62" s="7"/>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B63" s="7"/>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.35">
       <c r="B64" s="7"/>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B65" s="7"/>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B66" s="7"/>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B68" s="8"/>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B71" s="8"/>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B72" s="8"/>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B73" s="8"/>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B74" s="8"/>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B75" s="8"/>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B76" s="8"/>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B77" s="8"/>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B78" s="8"/>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B79" s="8"/>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B80" s="8"/>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B85" s="9"/>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B86" s="9"/>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B87" s="9"/>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B88" s="9"/>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B89" s="9"/>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B90" s="9"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
README.txt criado, parte do relatório feita, código comentado
</commit_message>
<xml_diff>
--- a/sd_checklist_meta1.xlsx
+++ b/sd_checklist_meta1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joao_\Documents\João Filipe\Universidade\4º Ano\2º Semestre\SD\Projeto-SD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07531BFC-4432-44A1-B5A4-DA19ADA95110}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26AA030-D548-4FFA-813C-853BA130CBE4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2016-2017" sheetId="2" r:id="rId1"/>
@@ -278,7 +278,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -288,12 +288,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -464,7 +458,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -491,9 +485,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -998,7 +989,7 @@
       <pane xSplit="2" ySplit="5" topLeftCell="C27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="B37" sqref="B37"/>
+      <selection pane="bottomRight" activeCell="B33" sqref="B33:C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.19921875" defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1060,7 +1051,7 @@
       <c r="A7" s="5">
         <v>1</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="5">
@@ -1071,7 +1062,7 @@
       <c r="A8" s="5">
         <v>3</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>39</v>
       </c>
       <c r="C8" s="5">
@@ -1082,7 +1073,7 @@
       <c r="A9" s="5">
         <v>3</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="11" t="s">
         <v>38</v>
       </c>
       <c r="C9" s="5">
@@ -1093,7 +1084,7 @@
       <c r="A10" s="5">
         <v>3</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>30</v>
       </c>
       <c r="C10" s="5">
@@ -1104,7 +1095,7 @@
       <c r="A11" s="5">
         <v>3</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="11" t="s">
         <v>40</v>
       </c>
       <c r="C11" s="5">
@@ -1115,7 +1106,7 @@
       <c r="A12" s="5">
         <v>3</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="11" t="s">
         <v>41</v>
       </c>
       <c r="C12" s="5">
@@ -1126,7 +1117,7 @@
       <c r="A13" s="5">
         <v>3</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="11" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="5">
@@ -1137,7 +1128,7 @@
       <c r="A14" s="5">
         <v>3</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="11" t="s">
         <v>31</v>
       </c>
       <c r="C14" s="5">
@@ -1148,7 +1139,7 @@
       <c r="A15" s="5">
         <v>3</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="11" t="s">
         <v>29</v>
       </c>
       <c r="C15" s="5">
@@ -1361,7 +1352,7 @@
       <c r="A34" s="5">
         <v>4</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C34" s="5">
@@ -1372,7 +1363,7 @@
       <c r="A35" s="5">
         <v>4</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="11" t="s">
         <v>44</v>
       </c>
       <c r="C35" s="5">
@@ -1383,7 +1374,7 @@
       <c r="A36" s="5">
         <v>4</v>
       </c>
-      <c r="B36" s="12" t="s">
+      <c r="B36" s="11" t="s">
         <v>6</v>
       </c>
       <c r="C36" s="5">

</xml_diff>